<commit_message>
simplecare row rates updated
</commit_message>
<xml_diff>
--- a/Inputs/Now_Health_SimpleCare_ROW/info.xlsx
+++ b/Inputs/Now_Health_SimpleCare_ROW/info.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">USD</t>
   </si>
   <si>
-    <t xml:space="preserve">Annual</t>
+    <t xml:space="preserve">Annually/month</t>
   </si>
   <si>
     <t xml:space="preserve">Now Health (Simple Care)</t>
@@ -206,10 +206,10 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>

</xml_diff>